<commit_message>
chinh sua logic sap xep cong viec ca nhan
</commit_message>
<xml_diff>
--- a/public/excels/Danh_sách_công_việc.xlsx
+++ b/public/excels/Danh_sách_công_việc.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="61">
   <si>
     <t>id</t>
   </si>
@@ -187,6 +187,21 @@
   </si>
   <si>
     <t>asdasDASDASDASDASDASDCZXCZXC</t>
+  </si>
+  <si>
+    <t>zxczx</t>
+  </si>
+  <si>
+    <t>2021-04-13</t>
+  </si>
+  <si>
+    <t>sczxc</t>
+  </si>
+  <si>
+    <t>2021-04-25</t>
+  </si>
+  <si>
+    <t>2021-04-27</t>
   </si>
 </sst>
 </file>
@@ -525,7 +540,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -1176,6 +1191,40 @@
         <v>30</v>
       </c>
       <c r="E38" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39">
+        <v>190</v>
+      </c>
+      <c r="B39" t="s">
+        <v>56</v>
+      </c>
+      <c r="C39" t="s">
+        <v>57</v>
+      </c>
+      <c r="D39" t="s">
+        <v>30</v>
+      </c>
+      <c r="E39" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40">
+        <v>191</v>
+      </c>
+      <c r="B40" t="s">
+        <v>58</v>
+      </c>
+      <c r="C40" t="s">
+        <v>59</v>
+      </c>
+      <c r="D40" t="s">
+        <v>60</v>
+      </c>
+      <c r="E40" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>

<commit_message>
chinh sua logic them anh ca nhan
</commit_message>
<xml_diff>
--- a/public/excels/Danh_sách_công_việc.xlsx
+++ b/public/excels/Danh_sách_công_việc.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="47">
   <si>
     <t>id</t>
   </si>
@@ -104,104 +104,58 @@
     <t>2021-04-12</t>
   </si>
   <si>
-    <t>mm</t>
+    <t>fix bug</t>
+  </si>
+  <si>
+    <t>2021-04-19</t>
+  </si>
+  <si>
+    <t>2021-04-20</t>
+  </si>
+  <si>
+    <t>dasdasdas</t>
   </si>
   <si>
     <t>2021-04-17</t>
   </si>
   <si>
-    <t>2021-04-30</t>
-  </si>
-  <si>
-    <t>di lam</t>
+    <t>2021-04-18</t>
+  </si>
+  <si>
+    <t>dsada</t>
+  </si>
+  <si>
+    <t>2021-04-13</t>
+  </si>
+  <si>
+    <t>Tạm dừng</t>
+  </si>
+  <si>
+    <t>asdasd</t>
+  </si>
+  <si>
+    <t>zcx</t>
+  </si>
+  <si>
+    <t>Chưa hoàn thành</t>
+  </si>
+  <si>
+    <t>di choi</t>
+  </si>
+  <si>
+    <t>2021-04-21</t>
+  </si>
+  <si>
+    <t>sadas</t>
   </si>
   <si>
     <t>2021-04-15</t>
   </si>
   <si>
-    <t>di choi</t>
-  </si>
-  <si>
-    <t>2021-04-14</t>
-  </si>
-  <si>
-    <t>2021-04-16</t>
-  </si>
-  <si>
-    <t>di hoc</t>
-  </si>
-  <si>
-    <t>di boi</t>
-  </si>
-  <si>
-    <t>2021-04-24</t>
-  </si>
-  <si>
-    <t>1. sadasdas
-2. 2ewdasdas</t>
-  </si>
-  <si>
-    <t>1:hung di choi
-2:hung di chocusd</t>
-  </si>
-  <si>
-    <t>sasdasd asd</t>
-  </si>
-  <si>
-    <t>Tạm dừng</t>
-  </si>
-  <si>
-    <t>asdas</t>
-  </si>
-  <si>
-    <t>ddddd</t>
-  </si>
-  <si>
-    <t>dasdas</t>
-  </si>
-  <si>
-    <t>Chưa hoàn thành</t>
-  </si>
-  <si>
-    <t>asdasd</t>
-  </si>
-  <si>
-    <t>sadas</t>
-  </si>
-  <si>
-    <t>1:di hoc</t>
-  </si>
-  <si>
-    <t>2:di choi</t>
-  </si>
-  <si>
-    <t>3:di boi</t>
-  </si>
-  <si>
-    <t>.</t>
-  </si>
-  <si>
-    <t>dasdasd
-12312
-asdasd</t>
-  </si>
-  <si>
-    <t>asdasDASDASDASDASDASDCZXCZXC</t>
-  </si>
-  <si>
-    <t>zxczx</t>
-  </si>
-  <si>
-    <t>2021-04-13</t>
-  </si>
-  <si>
-    <t>sczxc</t>
-  </si>
-  <si>
-    <t>2021-04-25</t>
-  </si>
-  <si>
-    <t>2021-04-27</t>
+    <t>vvvvvv</t>
+  </si>
+  <si>
+    <t>hung</t>
   </si>
 </sst>
 </file>
@@ -540,7 +494,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -814,7 +768,7 @@
         <v>33</v>
       </c>
       <c r="D16" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E16" t="s">
         <v>7</v>
@@ -825,30 +779,30 @@
         <v>163</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D17" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E17" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C18" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D18" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E18" t="s">
         <v>7</v>
@@ -856,19 +810,19 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C19" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D19" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="E19" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -876,16 +830,16 @@
         <v>170</v>
       </c>
       <c r="B20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" t="s">
+        <v>42</v>
+      </c>
+      <c r="E20" t="s">
         <v>40</v>
-      </c>
-      <c r="C20" t="s">
-        <v>19</v>
-      </c>
-      <c r="D20" t="s">
-        <v>33</v>
-      </c>
-      <c r="E20" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -893,16 +847,16 @@
         <v>171</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C21" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="D21" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E21" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -910,322 +864,33 @@
         <v>172</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C22" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D22" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="E22" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B23" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="C23" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="D23" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E23" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24">
-        <v>175</v>
-      </c>
-      <c r="B24" t="s">
-        <v>44</v>
-      </c>
-      <c r="C24" t="s">
-        <v>33</v>
-      </c>
-      <c r="D24" t="s">
-        <v>36</v>
-      </c>
-      <c r="E24" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25">
-        <v>176</v>
-      </c>
-      <c r="B25" t="s">
-        <v>44</v>
-      </c>
-      <c r="C25" t="s">
-        <v>33</v>
-      </c>
-      <c r="D25" t="s">
-        <v>33</v>
-      </c>
-      <c r="E25" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26">
-        <v>177</v>
-      </c>
-      <c r="B26" t="s">
-        <v>44</v>
-      </c>
-      <c r="C26" t="s">
-        <v>33</v>
-      </c>
-      <c r="D26" t="s">
-        <v>33</v>
-      </c>
-      <c r="E26" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27">
-        <v>178</v>
-      </c>
-      <c r="B27" t="s">
-        <v>45</v>
-      </c>
-      <c r="C27" t="s">
-        <v>33</v>
-      </c>
-      <c r="D27" t="s">
-        <v>33</v>
-      </c>
-      <c r="E27" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28">
-        <v>179</v>
-      </c>
-      <c r="B28" t="s">
-        <v>46</v>
-      </c>
-      <c r="C28" t="s">
-        <v>35</v>
-      </c>
-      <c r="D28" t="s">
-        <v>36</v>
-      </c>
-      <c r="E28" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29">
-        <v>180</v>
-      </c>
-      <c r="B29" t="s">
-        <v>48</v>
-      </c>
-      <c r="C29" t="s">
-        <v>35</v>
-      </c>
-      <c r="D29" t="s">
-        <v>36</v>
-      </c>
-      <c r="E29" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30">
-        <v>181</v>
-      </c>
-      <c r="B30" t="s">
-        <v>49</v>
-      </c>
-      <c r="C30" t="s">
-        <v>35</v>
-      </c>
-      <c r="D30" t="s">
-        <v>36</v>
-      </c>
-      <c r="E30" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31">
-        <v>182</v>
-      </c>
-      <c r="B31" t="s">
-        <v>48</v>
-      </c>
-      <c r="C31" t="s">
-        <v>35</v>
-      </c>
-      <c r="D31" t="s">
-        <v>36</v>
-      </c>
-      <c r="E31" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32">
-        <v>183</v>
-      </c>
-      <c r="B32" t="s">
-        <v>50</v>
-      </c>
-      <c r="C32" t="s">
-        <v>36</v>
-      </c>
-      <c r="D32" t="s">
-        <v>30</v>
-      </c>
-      <c r="E32" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33">
-        <v>184</v>
-      </c>
-      <c r="B33" t="s">
-        <v>51</v>
-      </c>
-      <c r="C33" t="s">
-        <v>36</v>
-      </c>
-      <c r="D33" t="s">
-        <v>30</v>
-      </c>
-      <c r="E33" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34">
-        <v>185</v>
-      </c>
-      <c r="B34" t="s">
-        <v>52</v>
-      </c>
-      <c r="C34" t="s">
-        <v>36</v>
-      </c>
-      <c r="D34" t="s">
-        <v>30</v>
-      </c>
-      <c r="E34" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35">
-        <v>186</v>
-      </c>
-      <c r="B35" t="s">
-        <v>34</v>
-      </c>
-      <c r="C35" t="s">
-        <v>33</v>
-      </c>
-      <c r="D35" t="s">
-        <v>30</v>
-      </c>
-      <c r="E35" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36">
-        <v>187</v>
-      </c>
-      <c r="B36" t="s">
-        <v>53</v>
-      </c>
-      <c r="C36" t="s">
-        <v>33</v>
-      </c>
-      <c r="D36" t="s">
-        <v>36</v>
-      </c>
-      <c r="E36" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37">
-        <v>188</v>
-      </c>
-      <c r="B37" t="s">
-        <v>54</v>
-      </c>
-      <c r="C37" t="s">
-        <v>33</v>
-      </c>
-      <c r="D37" t="s">
-        <v>36</v>
-      </c>
-      <c r="E37" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38">
-        <v>189</v>
-      </c>
-      <c r="B38" t="s">
-        <v>55</v>
-      </c>
-      <c r="C38" t="s">
-        <v>36</v>
-      </c>
-      <c r="D38" t="s">
-        <v>30</v>
-      </c>
-      <c r="E38" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39">
-        <v>190</v>
-      </c>
-      <c r="B39" t="s">
-        <v>56</v>
-      </c>
-      <c r="C39" t="s">
-        <v>57</v>
-      </c>
-      <c r="D39" t="s">
-        <v>30</v>
-      </c>
-      <c r="E39" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40">
-        <v>191</v>
-      </c>
-      <c r="B40" t="s">
-        <v>58</v>
-      </c>
-      <c r="C40" t="s">
-        <v>59</v>
-      </c>
-      <c r="D40" t="s">
-        <v>60</v>
-      </c>
-      <c r="E40" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update logic so lan qua han
</commit_message>
<xml_diff>
--- a/public/excels/Danh_sách_công_việc.xlsx
+++ b/public/excels/Danh_sách_công_việc.xlsx
@@ -137,19 +137,19 @@
     <t>zcx</t>
   </si>
   <si>
+    <t>di choi</t>
+  </si>
+  <si>
+    <t>2021-04-16</t>
+  </si>
+  <si>
+    <t>sadas</t>
+  </si>
+  <si>
+    <t>2021-04-15</t>
+  </si>
+  <si>
     <t>Chưa hoàn thành</t>
-  </si>
-  <si>
-    <t>di choi</t>
-  </si>
-  <si>
-    <t>2021-04-21</t>
-  </si>
-  <si>
-    <t>sadas</t>
-  </si>
-  <si>
-    <t>2021-04-15</t>
   </si>
   <si>
     <t>vvvvvv</t>
@@ -494,7 +494,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -519,86 +519,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3">
-        <v>40</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4">
-        <v>67</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5">
-        <v>85</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" t="s">
-        <v>7</v>
-      </c>
-    </row>
     <row r="6" spans="1:5">
       <c r="A6">
-        <v>92</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="E6" t="s">
         <v>7</v>
@@ -606,16 +538,16 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7">
-        <v>93</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E7" t="s">
         <v>7</v>
@@ -623,16 +555,16 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8">
-        <v>107</v>
+        <v>67</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E8" t="s">
         <v>7</v>
@@ -640,16 +572,16 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9">
-        <v>117</v>
+        <v>85</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E9" t="s">
         <v>7</v>
@@ -657,16 +589,16 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E10" t="s">
         <v>7</v>
@@ -674,16 +606,16 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E11" t="s">
         <v>7</v>
@@ -691,16 +623,16 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12">
-        <v>135</v>
+        <v>107</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E12" t="s">
         <v>7</v>
@@ -708,16 +640,16 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13">
-        <v>136</v>
+        <v>117</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D13" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E13" t="s">
         <v>7</v>
@@ -725,16 +657,16 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14">
-        <v>145</v>
+        <v>118</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D14" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E14" t="s">
         <v>7</v>
@@ -742,16 +674,16 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15">
-        <v>161</v>
+        <v>119</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="D15" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="E15" t="s">
         <v>7</v>
@@ -759,16 +691,16 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16">
-        <v>162</v>
+        <v>135</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="D16" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="E16" t="s">
         <v>7</v>
@@ -776,33 +708,33 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17">
-        <v>163</v>
+        <v>136</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C17" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="D17" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="E17" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18">
-        <v>168</v>
+        <v>145</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E18" t="s">
         <v>7</v>
@@ -810,87 +742,155 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="C19" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D19" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E19" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D20" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="E20" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C21" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D21" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E21" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C22" t="s">
         <v>30</v>
       </c>
       <c r="D22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E22" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23">
+        <v>169</v>
+      </c>
+      <c r="B23" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24">
+        <v>170</v>
+      </c>
+      <c r="B24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" t="s">
+        <v>41</v>
+      </c>
+      <c r="E24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25">
+        <v>171</v>
+      </c>
+      <c r="B25" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26">
+        <v>172</v>
+      </c>
+      <c r="B26" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" t="s">
+        <v>31</v>
+      </c>
+      <c r="E26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27">
         <v>173</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B27" t="s">
         <v>46</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C27" t="s">
         <v>25</v>
       </c>
-      <c r="D23" t="s">
-        <v>28</v>
-      </c>
-      <c r="E23" t="s">
-        <v>40</v>
+      <c r="D27" t="s">
+        <v>25</v>
+      </c>
+      <c r="E27" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update file the last time
</commit_message>
<xml_diff>
--- a/public/excels/Danh_sách_công_việc.xlsx
+++ b/public/excels/Danh_sách_công_việc.xlsx
@@ -7,15 +7,17 @@
     <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Worksheet" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <definedNames/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet1'!$A$1:$E$1</definedName>
+  </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="60">
   <si>
     <t>id</t>
   </si>
@@ -156,6 +158,45 @@
   </si>
   <si>
     <t>hung</t>
+  </si>
+  <si>
+    <t>czxc</t>
+  </si>
+  <si>
+    <t>2021-04-21</t>
+  </si>
+  <si>
+    <t>dasdddddd</t>
+  </si>
+  <si>
+    <t>vvvvv</t>
+  </si>
+  <si>
+    <t>bbbbb</t>
+  </si>
+  <si>
+    <t>dasd</t>
+  </si>
+  <si>
+    <t>2021-04-22</t>
+  </si>
+  <si>
+    <t>asdas</t>
+  </si>
+  <si>
+    <t>2021-04-25</t>
+  </si>
+  <si>
+    <t>di didiid</t>
+  </si>
+  <si>
+    <t>sadasd</t>
+  </si>
+  <si>
+    <t>fucking bitch</t>
+  </si>
+  <si>
+    <t>aaaaaaaaa</t>
   </si>
 </sst>
 </file>
@@ -169,7 +210,7 @@
       <i val="0"/>
       <strike val="0"/>
       <u val="none"/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
@@ -491,16 +532,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="4.451294" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="85.883789" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="12.69928" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="12.69928" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="18.590698" bestFit="true" customWidth="true" style="0"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
@@ -519,18 +567,86 @@
         <v>4</v>
       </c>
     </row>
+    <row r="2" spans="1:5">
+      <c r="A2">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>67</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>85</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+    </row>
     <row r="6" spans="1:5">
       <c r="A6">
-        <v>4</v>
+        <v>92</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E6" t="s">
         <v>7</v>
@@ -538,16 +654,16 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7">
-        <v>40</v>
+        <v>93</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E7" t="s">
         <v>7</v>
@@ -555,16 +671,16 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8">
-        <v>67</v>
+        <v>107</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E8" t="s">
         <v>7</v>
@@ -572,16 +688,16 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9">
-        <v>85</v>
+        <v>117</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E9" t="s">
         <v>7</v>
@@ -589,16 +705,16 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10">
-        <v>92</v>
+        <v>118</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D10" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E10" t="s">
         <v>7</v>
@@ -606,16 +722,16 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D11" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E11" t="s">
         <v>7</v>
@@ -623,16 +739,16 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12">
-        <v>107</v>
+        <v>135</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D12" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="E12" t="s">
         <v>7</v>
@@ -640,16 +756,16 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13">
-        <v>117</v>
+        <v>136</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D13" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E13" t="s">
         <v>7</v>
@@ -657,16 +773,16 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14">
-        <v>118</v>
+        <v>145</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="D14" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="E14" t="s">
         <v>7</v>
@@ -674,16 +790,16 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15">
-        <v>119</v>
+        <v>161</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="E15" t="s">
         <v>7</v>
@@ -691,16 +807,16 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16">
-        <v>135</v>
+        <v>162</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C16" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="D16" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="E16" t="s">
         <v>7</v>
@@ -708,33 +824,33 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17">
-        <v>136</v>
+        <v>163</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="C17" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D17" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="E17" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18">
-        <v>145</v>
+        <v>168</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="C18" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D18" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E18" t="s">
         <v>7</v>
@@ -742,16 +858,16 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="C19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" t="s">
         <v>30</v>
-      </c>
-      <c r="D19" t="s">
-        <v>31</v>
       </c>
       <c r="E19" t="s">
         <v>7</v>
@@ -759,16 +875,16 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="B20" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C20" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D20" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="E20" t="s">
         <v>7</v>
@@ -776,50 +892,50 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="B21" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C21" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="D21" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E21" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="B22" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="C22" t="s">
         <v>30</v>
       </c>
       <c r="D22" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E22" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="B23" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C23" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D23" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E23" t="s">
         <v>7</v>
@@ -827,30 +943,30 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="B24" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C24" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="D24" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="E24" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="B25" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="C25" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D25" t="s">
         <v>31</v>
@@ -861,16 +977,16 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="B26" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C26" t="s">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="D26" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E26" t="s">
         <v>44</v>
@@ -878,23 +994,143 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="B27" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C27" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="D27" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="E27" t="s">
-        <v>7</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28">
+        <v>180</v>
+      </c>
+      <c r="B28" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" t="s">
+        <v>31</v>
+      </c>
+      <c r="D28" t="s">
+        <v>53</v>
+      </c>
+      <c r="E28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29">
+        <v>181</v>
+      </c>
+      <c r="B29" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" t="s">
+        <v>55</v>
+      </c>
+      <c r="E29" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30">
+        <v>182</v>
+      </c>
+      <c r="B30" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" t="s">
+        <v>31</v>
+      </c>
+      <c r="D30" t="s">
+        <v>48</v>
+      </c>
+      <c r="E30" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31">
+        <v>183</v>
+      </c>
+      <c r="B31" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" t="s">
+        <v>31</v>
+      </c>
+      <c r="D31" t="s">
+        <v>48</v>
+      </c>
+      <c r="E31" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32">
+        <v>184</v>
+      </c>
+      <c r="B32" t="s">
+        <v>57</v>
+      </c>
+      <c r="C32" t="s">
+        <v>36</v>
+      </c>
+      <c r="D32" t="s">
+        <v>43</v>
+      </c>
+      <c r="E32" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33">
+        <v>185</v>
+      </c>
+      <c r="B33" t="s">
+        <v>58</v>
+      </c>
+      <c r="C33" t="s">
+        <v>36</v>
+      </c>
+      <c r="D33" t="s">
+        <v>33</v>
+      </c>
+      <c r="E33" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34">
+        <v>186</v>
+      </c>
+      <c r="B34" t="s">
+        <v>59</v>
+      </c>
+      <c r="C34" t="s">
+        <v>31</v>
+      </c>
+      <c r="D34" t="s">
+        <v>48</v>
+      </c>
+      <c r="E34" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <autoFilter ref="A1:E1"/>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
fix css bar chart
</commit_message>
<xml_diff>
--- a/public/excels/Danh_sách_công_việc.xlsx
+++ b/public/excels/Danh_sách_công_việc.xlsx
@@ -9176,7 +9176,7 @@
     </row>
     <row r="503" spans="1:7">
       <c r="A503" s="7">
-        <v>651</v>
+        <v>1651</v>
       </c>
       <c r="B503" s="7" t="s">
         <v>64</v>
@@ -9193,7 +9193,7 @@
     </row>
     <row r="504" spans="1:7">
       <c r="A504" s="7">
-        <v>652</v>
+        <v>1652</v>
       </c>
       <c r="B504" s="7" t="s">
         <v>64</v>
@@ -9210,7 +9210,7 @@
     </row>
     <row r="505" spans="1:7">
       <c r="A505" s="7">
-        <v>653</v>
+        <v>1653</v>
       </c>
       <c r="B505" s="7" t="s">
         <v>64</v>

</xml_diff>